<commit_message>
Update README with homonyms preview and fix visualizer
</commit_message>
<xml_diff>
--- a/workdir/resultados.xlsx
+++ b/workdir/resultados.xlsx
@@ -1886,15 +1886,23 @@
           <t>Kra 70 Nro 26A - 33</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>ZERO_RESULTS</t>
-        </is>
-      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Cra. 70 # 26A-33, Medellín, Belén, Medellín, Antioquia, Colombia</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>6.2286996</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-75.591641</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>ChIJr_BGq7gpRI4RTsUocgp2KDA</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr"/>
       <c r="G56" t="n">
         <v>100</v>
       </c>
@@ -1905,15 +1913,23 @@
           <t>Kra 70 Nro 26A 33</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>ZERO_RESULTS</t>
-        </is>
-      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Cra. 70 # 26A-33, Medellín, Belén, Medellín, Antioquia, Colombia</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>6.2286996</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-75.591641</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>ChIJr_BGq7gpRI4RTsUocgp2KDA</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
       <c r="G57" t="n">
         <v>100</v>
       </c>
@@ -1924,15 +1940,23 @@
           <t>Kra 70 Num 26A - 33</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>ZERO_RESULTS</t>
-        </is>
-      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Cra. 70 # 26A-33, Medellín, Belén, Medellín, Antioquia, Colombia</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>6.2286996</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-75.591641</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>ChIJr_BGq7gpRI4RTsUocgp2KDA</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
       <c r="G58" t="n">
         <v>100</v>
       </c>
@@ -1943,15 +1967,23 @@
           <t>Kra 70 Num 26A 33</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>ZERO_RESULTS</t>
-        </is>
-      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Cra. 70 # 26A-33, Medellín, Belén, Medellín, Antioquia, Colombia</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>6.2286996</v>
+      </c>
+      <c r="D59" t="n">
+        <v>-75.591641</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>ChIJr_BGq7gpRI4RTsUocgp2KDA</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
       <c r="G59" t="n">
         <v>100</v>
       </c>
@@ -1962,15 +1994,23 @@
           <t>Kra 70 Numero 26A - 33</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>ZERO_RESULTS</t>
-        </is>
-      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Cra. 70 # 26A-33, Medellín, Belén, Medellín, Antioquia, Colombia</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>6.2286996</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-75.591641</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>ChIJr_BGq7gpRI4RTsUocgp2KDA</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr"/>
       <c r="G60" t="n">
         <v>100</v>
       </c>
@@ -1981,15 +2021,23 @@
           <t>Kra 70 Numero 26A 33</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>ZERO_RESULTS</t>
-        </is>
-      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Cra. 70 # 26A-33, Medellín, Belén, Medellín, Antioquia, Colombia</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>6.2286996</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-75.591641</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>ChIJr_BGq7gpRI4RTsUocgp2KDA</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr"/>
       <c r="G61" t="n">
         <v>100</v>
       </c>

</xml_diff>